<commit_message>
new changes from nov month
</commit_message>
<xml_diff>
--- a/src/test/java/com/hpeb2c/testData/testdata.xlsx
+++ b/src/test/java/com/hpeb2c/testData/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ritesh\HPE_B2C\src\test\java\com\hpeb2c\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F6D209-209A-467A-9E2B-78F7078FC7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8294AB1-6200-4F17-8DE5-3B4FCED83E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
     <t>Invalid</t>
   </si>
   <si>
-    <t>sanitycheck9250@yopmail.com</t>
+    <t>sanitycheck9150@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -480,8 +480,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F5D0DE3F-DAC4-4AC9-9792-B1894D68A35A}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{E0FA41F3-4F53-4FE7-95D5-4677CFFACFE9}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E0FA41F3-4F53-4FE7-95D5-4677CFFACFE9}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{5F4A56F4-3AB2-430B-9048-BCE2F762A205}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>